<commit_message>
Added Security working code
</commit_message>
<xml_diff>
--- a/src/main/resources/users.xlsx
+++ b/src/main/resources/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51CC54D4-E225-4FC9-B183-517568B9EAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{565BE603-403C-4F47-8459-95A0E97A5593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Id</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>$2a$12$4tuF4ECM63Ax3dEqBECu/.HsGl6nvUB7U0qs/nqRNzMv26i.6giWS</t>
+  </si>
+  <si>
+    <t>ADMIN,STAFF</t>
+  </si>
+  <si>
+    <t>pqr</t>
+  </si>
+  <si>
+    <t>$2a$12$Z6brAIjlD7Tu6/3ST2c3aO/M4vpE40UWRIM8wQIfTxq76De7bMhku</t>
+  </si>
+  <si>
+    <t>mno</t>
+  </si>
+  <si>
+    <t>$2a$12$VSmfazM8wxdzTyNEnEF6pOD5lAcreSIGTsrkVtnYv382ZBlJRoaQ6</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,15 +601,43 @@
         <v>45545</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>4.0</v>
+    <row r="5" spans="1:7">
+      <c r="A5" s="0">
+        <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>21</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>